<commit_message>
Flos Tabelle unten angehängt
</commit_message>
<xml_diff>
--- a/src/praktikum4/tabelle BSP.xlsx
+++ b/src/praktikum4/tabelle BSP.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Files\Dropbox\Dropbox\Uni\Semester 3\Betriebssysteme\Höling\VirtualMemory-Vorgabecode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\Linux\BSP\src\praktikum4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23430" windowHeight="8940"/>
+    <workbookView xWindow="1110" yWindow="0" windowWidth="23430" windowHeight="8940"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="10">
   <si>
     <t>MAX_RAM_PAGES_ PER_PROCESS (Hauptspeicherzuteilung)</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>clock zu fifo</t>
+  </si>
+  <si>
+    <t>Florians Lösung</t>
   </si>
 </sst>
 </file>
@@ -97,6 +100,7 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -106,12 +110,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -144,11 +147,31 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -164,11 +187,21 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -482,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:K13"/>
+  <dimension ref="B6:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,21 +530,21 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="I6" t="s">
@@ -525,13 +558,13 @@
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
       <c r="I7" t="s">
         <v>5</v>
       </c>
@@ -543,14 +576,14 @@
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="1">
-        <v>10</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1">
+      <c r="B8" s="2">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2">
         <v>1</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="2"/>
       <c r="F8">
         <v>0.54350924</v>
       </c>
@@ -560,28 +593,28 @@
       <c r="H8">
         <v>0.47258484000000001</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="1">
         <f>F8/G8</f>
         <v>1.0965537384815647</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="1">
         <f>F8/H8</f>
         <v>1.1500776029971675</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="1">
         <f>G8/H8</f>
         <v>1.0488109817488009</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="1">
-        <v>10</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1">
-        <v>10</v>
-      </c>
-      <c r="E9" s="1"/>
+      <c r="B9" s="2">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2">
+        <v>10</v>
+      </c>
+      <c r="E9" s="2"/>
       <c r="F9">
         <v>0.51738523999999997</v>
       </c>
@@ -591,28 +624,28 @@
       <c r="H9">
         <v>0.48531289999999999</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="1">
         <f t="shared" ref="I9:I13" si="0">F9/G9</f>
         <v>1.0165919854348509</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="1">
         <f t="shared" ref="J9:J13" si="1">F9/H9</f>
         <v>1.0660859004572101</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="1">
         <f t="shared" ref="K9:K13" si="2">G9/H9</f>
         <v>1.0486861156997889</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="1">
-        <v>10</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1">
+      <c r="B10" s="2">
+        <v>10</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2">
         <v>100</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="2"/>
       <c r="F10">
         <v>0.48806366000000001</v>
       </c>
@@ -622,28 +655,28 @@
       <c r="H10">
         <v>0.49737049999999999</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="1">
         <f t="shared" si="0"/>
         <v>0.94553235148990078</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="1">
         <f t="shared" si="1"/>
         <v>0.98128791313517794</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="1">
         <f t="shared" si="2"/>
         <v>1.0378152705075994</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="1">
-        <v>10</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1">
+      <c r="B11" s="2">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2">
         <v>1000</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="2"/>
       <c r="F11">
         <v>0.5116598</v>
       </c>
@@ -653,28 +686,28 @@
       <c r="H11">
         <v>0.49339149999999998</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="1">
         <f t="shared" si="0"/>
         <v>0.95879939963985505</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="1">
         <f t="shared" si="1"/>
         <v>1.0370259722755661</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="1">
         <f t="shared" si="2"/>
         <v>1.0815880492468963</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="1">
+      <c r="B12" s="2">
         <v>15</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1">
-        <v>10</v>
-      </c>
-      <c r="E12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2">
+        <v>10</v>
+      </c>
+      <c r="E12" s="2"/>
       <c r="F12">
         <v>0.50476193000000003</v>
       </c>
@@ -684,28 +717,28 @@
       <c r="H12">
         <v>0.50145410000000001</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="1">
         <f t="shared" si="0"/>
         <v>1.0277134842839599</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="1">
         <f t="shared" si="1"/>
         <v>1.0065964761281243</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="1">
         <f t="shared" si="2"/>
         <v>0.97945243642439062</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="1">
+      <c r="B13" s="2">
         <v>20</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1">
-        <v>10</v>
-      </c>
-      <c r="E13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2">
+        <v>10</v>
+      </c>
+      <c r="E13" s="2"/>
       <c r="F13">
         <v>0.50407606000000005</v>
       </c>
@@ -715,21 +748,282 @@
       <c r="H13">
         <v>0.51527226000000004</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="1">
         <f t="shared" si="0"/>
         <v>0.99109108168346816</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13" s="1">
         <f t="shared" si="1"/>
         <v>0.97827129292774273</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K13" s="1">
         <f t="shared" si="2"/>
         <v>0.98706497415560468</v>
       </c>
     </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" t="s">
+        <v>7</v>
+      </c>
+      <c r="J16" t="s">
+        <v>7</v>
+      </c>
+      <c r="K16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J17" t="s">
+        <v>6</v>
+      </c>
+      <c r="K17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
+        <v>10</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18">
+        <v>0.49</v>
+      </c>
+      <c r="G18">
+        <v>0.48349999999999999</v>
+      </c>
+      <c r="H18">
+        <v>0.4874</v>
+      </c>
+      <c r="I18" s="1">
+        <f>F18/G18</f>
+        <v>1.0134436401240952</v>
+      </c>
+      <c r="J18" s="1">
+        <f>F18/H18</f>
+        <v>1.0053344275748872</v>
+      </c>
+      <c r="K18" s="1">
+        <f>G18/H18</f>
+        <v>0.99199835863766928</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="2">
+        <v>10</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2">
+        <v>10</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19">
+        <v>0.51659999999999995</v>
+      </c>
+      <c r="G19">
+        <v>0.49</v>
+      </c>
+      <c r="H19">
+        <v>0.49</v>
+      </c>
+      <c r="I19" s="1">
+        <f t="shared" ref="I19:I23" si="3">F19/G19</f>
+        <v>1.0542857142857143</v>
+      </c>
+      <c r="J19" s="1">
+        <f t="shared" ref="J19:J23" si="4">F19/H19</f>
+        <v>1.0542857142857143</v>
+      </c>
+      <c r="K19" s="1">
+        <f t="shared" ref="K19:K23" si="5">G19/H19</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
+        <v>10</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2">
+        <v>100</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20">
+        <v>0.49671999999999999</v>
+      </c>
+      <c r="G20">
+        <v>0.47549999999999998</v>
+      </c>
+      <c r="H20">
+        <v>0.48020000000000002</v>
+      </c>
+      <c r="I20" s="1">
+        <f t="shared" si="3"/>
+        <v>1.0446267087276551</v>
+      </c>
+      <c r="J20" s="1">
+        <f t="shared" si="4"/>
+        <v>1.0344023323615159</v>
+      </c>
+      <c r="K20" s="1">
+        <f t="shared" si="5"/>
+        <v>0.99021241149521022</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="2">
+        <v>10</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21">
+        <v>0.49409999999999998</v>
+      </c>
+      <c r="G21">
+        <v>0.50929999999999997</v>
+      </c>
+      <c r="H21">
+        <v>0.48549999999999999</v>
+      </c>
+      <c r="I21" s="1">
+        <f t="shared" si="3"/>
+        <v>0.97015511486353823</v>
+      </c>
+      <c r="J21" s="1">
+        <f t="shared" si="4"/>
+        <v>1.0177136972193614</v>
+      </c>
+      <c r="K21" s="1">
+        <f t="shared" si="5"/>
+        <v>1.0490216271884654</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="2">
+        <v>15</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2">
+        <v>10</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22">
+        <v>0.52</v>
+      </c>
+      <c r="G22">
+        <v>0.51980000000000004</v>
+      </c>
+      <c r="H22">
+        <v>0.49280000000000002</v>
+      </c>
+      <c r="I22" s="1">
+        <f t="shared" si="3"/>
+        <v>1.0003847633705272</v>
+      </c>
+      <c r="J22" s="1">
+        <f t="shared" si="4"/>
+        <v>1.0551948051948052</v>
+      </c>
+      <c r="K22" s="1">
+        <f t="shared" si="5"/>
+        <v>1.0547889610389611</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="2">
+        <v>20</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2">
+        <v>10</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23">
+        <v>0.4824</v>
+      </c>
+      <c r="G23">
+        <v>0.48709999999999998</v>
+      </c>
+      <c r="H23">
+        <v>0.48370000000000002</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" si="3"/>
+        <v>0.9903510572777664</v>
+      </c>
+      <c r="J23" s="1">
+        <f t="shared" si="4"/>
+        <v>0.9973123837089104</v>
+      </c>
+      <c r="K23" s="1">
+        <f t="shared" si="5"/>
+        <v>1.0070291502997726</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="34">
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="D16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="B6:C7"/>
+    <mergeCell ref="D6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="B13:C13"/>
@@ -740,22 +1034,26 @@
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B6:C7"/>
-    <mergeCell ref="D6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
   </mergeCells>
   <conditionalFormatting sqref="I8:K13">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18:K23">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Praktikum 4 Kommentare vom Prof
</commit_message>
<xml_diff>
--- a/src/praktikum4/tabelle BSP.xlsx
+++ b/src/praktikum4/tabelle BSP.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3330" yWindow="0" windowWidth="23430" windowHeight="8940"/>
+    <workbookView xWindow="4440" yWindow="0" windowWidth="23430" windowHeight="8940"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="17">
   <si>
     <t>MAX_RAM_PAGES_ PER_PROCESS (Hauptspeicherzuteilung)</t>
   </si>
@@ -63,14 +63,94 @@
   </si>
   <si>
     <t>praktikum 4_2</t>
+  </si>
+  <si>
+    <t>Programm ist 20 Seiten groß --&gt; mit max_20 Seiten braucht der Prozess nichts mehr laden --&gt; keine seitenfehler</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>clock</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> zu fifo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rand</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> zu fifo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rand</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> zu clock</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -110,14 +190,14 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -524,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A6:K32"/>
+  <dimension ref="A6:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,21 +623,21 @@
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="I6" t="s">
@@ -571,13 +651,13 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
       <c r="I7" t="s">
         <v>5</v>
       </c>
@@ -589,14 +669,14 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="4">
-        <v>10</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4">
+      <c r="B8" s="2">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2">
         <v>1</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="2"/>
       <c r="F8">
         <v>0.54350924</v>
       </c>
@@ -620,14 +700,14 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="4">
-        <v>10</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4">
-        <v>10</v>
-      </c>
-      <c r="E9" s="4"/>
+      <c r="B9" s="2">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2">
+        <v>10</v>
+      </c>
+      <c r="E9" s="2"/>
       <c r="F9">
         <v>0.51738523999999997</v>
       </c>
@@ -651,14 +731,14 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="4">
-        <v>10</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4">
+      <c r="B10" s="2">
+        <v>10</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2">
         <v>100</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="2"/>
       <c r="F10">
         <v>0.48806366000000001</v>
       </c>
@@ -682,14 +762,14 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="4">
-        <v>10</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4">
+      <c r="B11" s="2">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2">
         <v>1000</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="E11" s="2"/>
       <c r="F11">
         <v>0.5116598</v>
       </c>
@@ -713,14 +793,14 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="4">
+      <c r="B12" s="2">
         <v>15</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4">
-        <v>10</v>
-      </c>
-      <c r="E12" s="4"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2">
+        <v>10</v>
+      </c>
+      <c r="E12" s="2"/>
       <c r="F12">
         <v>0.50476193000000003</v>
       </c>
@@ -744,14 +824,14 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="4">
+      <c r="B13" s="2">
         <v>20</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4">
-        <v>10</v>
-      </c>
-      <c r="E13" s="4"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2">
+        <v>10</v>
+      </c>
+      <c r="E13" s="2"/>
       <c r="F13">
         <v>0.50407606000000005</v>
       </c>
@@ -783,21 +863,21 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2" t="s">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2" t="s">
+      <c r="E16" s="3"/>
+      <c r="F16" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="3" t="s">
         <v>4</v>
       </c>
       <c r="I16" t="s">
@@ -811,13 +891,13 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
       <c r="I17" t="s">
         <v>5</v>
       </c>
@@ -829,14 +909,14 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="4">
-        <v>10</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4">
+      <c r="B18" s="2">
+        <v>10</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2">
         <v>1</v>
       </c>
-      <c r="E18" s="4"/>
+      <c r="E18" s="2"/>
       <c r="F18">
         <v>0.43846153999999998</v>
       </c>
@@ -860,14 +940,14 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="4">
-        <v>10</v>
-      </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4">
-        <v>10</v>
-      </c>
-      <c r="E19" s="4"/>
+      <c r="B19" s="2">
+        <v>10</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2">
+        <v>10</v>
+      </c>
+      <c r="E19" s="2"/>
       <c r="F19">
         <v>0.23319968999999999</v>
       </c>
@@ -891,14 +971,14 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="4">
-        <v>10</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4">
+      <c r="B20" s="2">
+        <v>10</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2">
         <v>100</v>
       </c>
-      <c r="E20" s="4"/>
+      <c r="E20" s="2"/>
       <c r="F20">
         <v>3.0286897E-2</v>
       </c>
@@ -922,14 +1002,14 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="4">
-        <v>10</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4">
+      <c r="B21" s="2">
+        <v>10</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2">
         <v>1000</v>
       </c>
-      <c r="E21" s="4"/>
+      <c r="E21" s="2"/>
       <c r="F21">
         <v>3.6041939999999998E-3</v>
       </c>
@@ -953,14 +1033,14 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="4">
+      <c r="B22" s="2">
         <v>15</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4">
-        <v>10</v>
-      </c>
-      <c r="E22" s="4"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2">
+        <v>10</v>
+      </c>
+      <c r="E22" s="2"/>
       <c r="F22">
         <v>0.11202361399999999</v>
       </c>
@@ -984,14 +1064,14 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="4">
+      <c r="B23" s="2">
         <v>20</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4">
-        <v>10</v>
-      </c>
-      <c r="E23" s="4"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2">
+        <v>10</v>
+      </c>
+      <c r="E23" s="2"/>
       <c r="F23">
         <v>0</v>
       </c>
@@ -1018,21 +1098,21 @@
       <c r="A25" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2" t="s">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2" t="s">
+      <c r="E25" s="3"/>
+      <c r="F25" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="H25" s="3" t="s">
         <v>4</v>
       </c>
       <c r="I25" t="s">
@@ -1046,32 +1126,32 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
       <c r="I26" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="J26" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="K26" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="4">
-        <v>10</v>
-      </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4">
+      <c r="B27" s="2">
+        <v>10</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2">
         <v>1</v>
       </c>
-      <c r="E27" s="4"/>
+      <c r="E27" s="2"/>
       <c r="F27">
         <v>0.5027741</v>
       </c>
@@ -1095,14 +1175,14 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="4">
-        <v>10</v>
-      </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4">
-        <v>10</v>
-      </c>
-      <c r="E28" s="4"/>
+      <c r="B28" s="2">
+        <v>10</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2">
+        <v>10</v>
+      </c>
+      <c r="E28" s="2"/>
       <c r="F28">
         <v>0.22178745</v>
       </c>
@@ -1126,14 +1206,14 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="4">
-        <v>10</v>
-      </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4">
+      <c r="B29" s="2">
+        <v>10</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2">
         <v>100</v>
       </c>
-      <c r="E29" s="4"/>
+      <c r="E29" s="2"/>
       <c r="F29">
         <v>3.1901529999999997E-2</v>
       </c>
@@ -1157,14 +1237,14 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="4">
-        <v>10</v>
-      </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4">
+      <c r="B30" s="2">
+        <v>10</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2">
         <v>1000</v>
       </c>
-      <c r="E30" s="4"/>
+      <c r="E30" s="2"/>
       <c r="F30">
         <v>3.7825361E-3</v>
       </c>
@@ -1183,19 +1263,19 @@
         <v>1.4650282030245951</v>
       </c>
       <c r="K30" s="1">
-        <f t="shared" si="8"/>
+        <f>G30/H30</f>
         <v>0.84149859122373405</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="4">
+      <c r="B31" s="2">
         <v>15</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4">
-        <v>10</v>
-      </c>
-      <c r="E31" s="4"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2">
+        <v>10</v>
+      </c>
+      <c r="E31" s="2"/>
       <c r="F31">
         <v>0.11058438600000001</v>
       </c>
@@ -1219,14 +1299,14 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="4">
+      <c r="B32" s="2">
         <v>20</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4">
-        <v>10</v>
-      </c>
-      <c r="E32" s="4"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2">
+        <v>10</v>
+      </c>
+      <c r="E32" s="2"/>
       <c r="F32">
         <v>0</v>
       </c>
@@ -1249,39 +1329,18 @@
         <v>#DIV/0!</v>
       </c>
     </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B25:C26"/>
-    <mergeCell ref="D25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B6:C7"/>
+    <mergeCell ref="D6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="B16:C17"/>
@@ -1297,11 +1356,37 @@
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B6:C7"/>
-    <mergeCell ref="D6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="B25:C26"/>
+    <mergeCell ref="D25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
   </mergeCells>
   <conditionalFormatting sqref="I8:K13">
     <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">

</xml_diff>